<commit_message>
Modified notebook to generate daily plot, removed count of swabs. Added plots dir
</commit_message>
<xml_diff>
--- a/data/covid-19_IT.xlsx
+++ b/data/covid-19_IT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlotorniai/repos/COVID-19-Italy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8000B6-2B0A-9940-8E1B-611E28C1CD1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229EFA46-2203-FA40-A687-0ED56DEE0B47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="460" windowWidth="17740" windowHeight="16660" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="460" windowWidth="17740" windowHeight="16660" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="23.02" sheetId="2" r:id="rId1"/>
@@ -545,7 +545,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -729,18 +729,13 @@
       <c r="G23" s="9">
         <v>2</v>
       </c>
-      <c r="H23" s="10">
-        <f>SUM(H2:H22)</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="9">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="H23" s="10"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="25" spans="1:9" ht="16">
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" ht="16">
       <c r="D26" s="1"/>
     </row>
   </sheetData>
@@ -760,7 +755,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -945,16 +940,10 @@
       <c r="G23" s="9">
         <v>6</v>
       </c>
-      <c r="H23" s="10">
-        <f t="shared" ref="H23:I23" si="0">SUM(H2:H22)</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+    </row>
+    <row r="25" spans="1:9" ht="16">
       <c r="E25" s="11"/>
     </row>
   </sheetData>
@@ -970,7 +959,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1165,16 +1154,10 @@
       <c r="G23" s="8">
         <v>10</v>
       </c>
-      <c r="H23" s="10">
-        <f t="shared" ref="H23:I23" si="0">SUM(H2:H22)</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+    </row>
+    <row r="25" spans="1:9" ht="16">
       <c r="E25" s="13"/>
     </row>
   </sheetData>
@@ -1190,7 +1173,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1390,16 +1373,10 @@
       <c r="G23" s="8">
         <v>12</v>
       </c>
-      <c r="H23" s="10">
-        <f t="shared" ref="H23:I23" si="0">SUM(H2:H22)</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+    </row>
+    <row r="25" spans="1:9" ht="16">
       <c r="E25" s="13"/>
     </row>
   </sheetData>
@@ -1415,7 +1392,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1623,16 +1600,10 @@
       <c r="G23" s="8">
         <v>17</v>
       </c>
-      <c r="H23" s="10">
-        <f t="shared" ref="H23:I23" si="0">SUM(H2:H22)</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+    </row>
+    <row r="25" spans="1:9" ht="16">
       <c r="E25" s="13"/>
     </row>
   </sheetData>
@@ -1644,7 +1615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -3151,7 +3122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -4772,7 +4743,7 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5015,7 +4986,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" ht="18">
       <c r="A9" s="15" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Added detailed data on the 27th and related screenshots
</commit_message>
<xml_diff>
--- a/data/covid-19_IT.xlsx
+++ b/data/covid-19_IT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlotorniai/repos/COVID-19-Italy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229EFA46-2203-FA40-A687-0ED56DEE0B47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06AC405-B8E1-0E41-9956-416AD25B16B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="460" windowWidth="17740" windowHeight="16660" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="460" windowWidth="17740" windowHeight="16660" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="23.02" sheetId="2" r:id="rId1"/>
@@ -134,7 +134,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -230,6 +230,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -288,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -321,6 +327,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1173,7 +1180,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="B2" sqref="B2:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1391,8 +1398,8 @@
   </sheetPr>
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1402,6 +1409,7 @@
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16">
@@ -1437,64 +1445,194 @@
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="B2">
+        <v>172</v>
+      </c>
+      <c r="C2">
+        <v>41</v>
+      </c>
+      <c r="D2">
+        <v>136</v>
+      </c>
       <c r="E2" s="1">
+        <f>SUM(B2:D2)</f>
+        <v>349</v>
+      </c>
+      <c r="F2">
+        <v>40</v>
+      </c>
+      <c r="G2">
+        <v>14</v>
+      </c>
+      <c r="H2">
+        <f>SUM(E2:G2)</f>
         <v>403</v>
+      </c>
+      <c r="I2">
+        <v>3320</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="B3">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>82</v>
+      </c>
       <c r="E3" s="1">
+        <f t="shared" ref="E3:E14" si="0">SUM(B3:D3)</f>
+        <v>109</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H22" si="1">SUM(E3:G3)</f>
         <v>111</v>
+      </c>
+      <c r="I3">
+        <v>6164</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="B4">
+        <v>36</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>54</v>
+      </c>
       <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
         <v>97</v>
+      </c>
+      <c r="I4">
+        <v>1033</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
       <c r="E5" s="1">
+        <f t="shared" si="0"/>
         <v>19</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="I5">
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
       <c r="E6" s="1">
+        <f t="shared" si="0"/>
         <v>2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
       <c r="E7" s="1">
+        <f t="shared" si="0"/>
         <v>2</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>410</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
       <c r="E8" s="1">
+        <f t="shared" si="0"/>
         <v>3</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="26">
+        <v>1</v>
+      </c>
       <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
         <v>4</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1">
@@ -1502,22 +1640,55 @@
         <v>16</v>
       </c>
       <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
         <v>3</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <v>552</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="D11" s="26">
+        <v>1</v>
+      </c>
       <c r="E11" s="1">
+        <f t="shared" si="0"/>
         <v>3</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="B12" s="26">
+        <v>1</v>
+      </c>
       <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1525,57 +1696,129 @@
       <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
       <c r="E13" s="1">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B14" s="26">
+        <v>1</v>
+      </c>
       <c r="E14" s="1">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1">
       <c r="A15" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1">
       <c r="A16" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1">
       <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>8</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1">
       <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>9</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1">
       <c r="A19" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>141</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1">
       <c r="A20" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>32</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1">
       <c r="A21" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1">
       <c r="A22" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1">
       <c r="A23" s="6" t="s">
@@ -1592,16 +1835,24 @@
       </c>
       <c r="E23" s="10">
         <f>SUM(E2:E22)</f>
+        <v>588</v>
+      </c>
+      <c r="F23" s="10">
+        <f>SUM(F2:F22)</f>
+        <v>45</v>
+      </c>
+      <c r="G23" s="10">
+        <f>SUM(G2:G22)</f>
+        <v>17</v>
+      </c>
+      <c r="H23" s="10">
+        <f>SUM(H2:H22)</f>
         <v>650</v>
       </c>
-      <c r="F23" s="8">
-        <v>45</v>
-      </c>
-      <c r="G23" s="8">
-        <v>17</v>
-      </c>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
+      <c r="I23" s="10">
+        <f>SUM(I2:I22)</f>
+        <v>12014</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="16">
       <c r="E25" s="13"/>
@@ -3122,7 +3373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updateed files, processed files and plots on 02.03 data
</commit_message>
<xml_diff>
--- a/data/covid-19_IT.xlsx
+++ b/data/covid-19_IT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlotorniai/repos/COVID-19-Italy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06AC405-B8E1-0E41-9956-416AD25B16B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3CB642-7B92-FC4C-8E97-19E087881742}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="460" windowWidth="17740" windowHeight="16660" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="460" windowWidth="17740" windowHeight="16660" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="23.02" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="27.02" sheetId="6" r:id="rId5"/>
     <sheet name="28.02" sheetId="7" r:id="rId6"/>
     <sheet name="29.02" sheetId="8" r:id="rId7"/>
-    <sheet name="1.03" sheetId="9" r:id="rId8"/>
+    <sheet name="01.03" sheetId="9" r:id="rId8"/>
+    <sheet name="02.03" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="31">
   <si>
     <t>Ricoverati con sintomi</t>
   </si>
@@ -1398,7 +1399,7 @@
   </sheetPr>
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -4998,7 +4999,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" sqref="A1:I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -5604,4 +5605,627 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B6AAFFF-DBD2-4D48-B9B2-FDF15311057D}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16">
+      <c r="A1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1">
+      <c r="A2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="19">
+        <v>478</v>
+      </c>
+      <c r="C2" s="19">
+        <v>127</v>
+      </c>
+      <c r="D2" s="19">
+        <v>472</v>
+      </c>
+      <c r="E2" s="16">
+        <f t="shared" ref="E2:E23" si="0">SUM(B2:D2)</f>
+        <v>1077</v>
+      </c>
+      <c r="F2" s="19">
+        <v>139</v>
+      </c>
+      <c r="G2" s="19">
+        <v>38</v>
+      </c>
+      <c r="H2" s="16">
+        <f t="shared" ref="H2:H22" si="1">SUM(E2:G2)</f>
+        <v>1254</v>
+      </c>
+      <c r="I2" s="19">
+        <v>7925</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1">
+      <c r="A3" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="19">
+        <v>53</v>
+      </c>
+      <c r="C3" s="19">
+        <v>14</v>
+      </c>
+      <c r="D3" s="19">
+        <v>204</v>
+      </c>
+      <c r="E3" s="16">
+        <f t="shared" si="0"/>
+        <v>271</v>
+      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16">
+        <v>2</v>
+      </c>
+      <c r="H3" s="16">
+        <f t="shared" si="1"/>
+        <v>273</v>
+      </c>
+      <c r="I3" s="19">
+        <v>9782</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1">
+      <c r="A4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="19">
+        <v>148</v>
+      </c>
+      <c r="C4" s="19">
+        <v>16</v>
+      </c>
+      <c r="D4" s="19">
+        <v>160</v>
+      </c>
+      <c r="E4" s="16">
+        <f t="shared" si="0"/>
+        <v>324</v>
+      </c>
+      <c r="F4" s="16"/>
+      <c r="G4" s="19">
+        <v>11</v>
+      </c>
+      <c r="H4" s="16">
+        <f t="shared" si="1"/>
+        <v>335</v>
+      </c>
+      <c r="I4" s="19">
+        <v>1973</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1">
+      <c r="A5" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="19">
+        <v>12</v>
+      </c>
+      <c r="C5" s="19">
+        <v>2</v>
+      </c>
+      <c r="D5" s="19">
+        <v>37</v>
+      </c>
+      <c r="E5" s="16">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="I5" s="19">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1">
+      <c r="A6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="19">
+        <v>12</v>
+      </c>
+      <c r="C6" s="16">
+        <v>1</v>
+      </c>
+      <c r="D6" s="19">
+        <v>5</v>
+      </c>
+      <c r="E6" s="16">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F6" s="16">
+        <v>4</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="I6" s="16">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1">
+      <c r="A7" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="19">
+        <v>17</v>
+      </c>
+      <c r="C7" s="19">
+        <v>6</v>
+      </c>
+      <c r="D7" s="19">
+        <v>11</v>
+      </c>
+      <c r="E7" s="16">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16">
+        <v>1</v>
+      </c>
+      <c r="H7" s="16">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="I7" s="19">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1">
+      <c r="A8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="16">
+        <v>7</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="19">
+        <v>5</v>
+      </c>
+      <c r="E8" s="16">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F8" s="16">
+        <v>1</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="I8" s="19">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18">
+      <c r="A9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="16">
+        <v>2</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="19">
+        <v>3</v>
+      </c>
+      <c r="E9" s="16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F9" s="16">
+        <v>2</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I9" s="19">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1">
+      <c r="A10" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="16">
+        <v>3</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16">
+        <v>1</v>
+      </c>
+      <c r="E10" s="16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F10" s="16">
+        <v>3</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I10" s="19">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1">
+      <c r="A11" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="19">
+        <v>4</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="19">
+        <v>13</v>
+      </c>
+      <c r="E11" s="16">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="I11" s="16">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1">
+      <c r="A12" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="16">
+        <v>2</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16">
+        <v>2</v>
+      </c>
+      <c r="E12" s="16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I12" s="19">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1">
+      <c r="A13" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="16">
+        <v>1</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I13" s="19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1">
+      <c r="A14" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="19">
+        <v>3</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="19">
+        <v>2</v>
+      </c>
+      <c r="E14" s="16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I14" s="19">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1">
+      <c r="A15" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16">
+        <v>1</v>
+      </c>
+      <c r="E15" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I15" s="19">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15" customHeight="1">
+      <c r="A16" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="19">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15" customHeight="1">
+      <c r="A17" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="19">
+        <v>2</v>
+      </c>
+      <c r="E17" s="16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I17" s="19">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" customHeight="1">
+      <c r="A18" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" customHeight="1">
+      <c r="A19" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="19">
+        <v>9</v>
+      </c>
+      <c r="E19" s="16">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I19" s="19">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" customHeight="1">
+      <c r="A20" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="19">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15" customHeight="1">
+      <c r="A21" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" customHeight="1" thickBot="1">
+      <c r="A22" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="19">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15" customHeight="1" thickBot="1">
+      <c r="A23" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="21">
+        <f t="shared" ref="B23:D23" si="2">SUM(B2:B22)</f>
+        <v>742</v>
+      </c>
+      <c r="C23" s="21">
+        <f t="shared" si="2"/>
+        <v>166</v>
+      </c>
+      <c r="D23" s="21">
+        <f t="shared" si="2"/>
+        <v>927</v>
+      </c>
+      <c r="E23" s="22">
+        <f t="shared" si="0"/>
+        <v>1835</v>
+      </c>
+      <c r="F23" s="22">
+        <f t="shared" ref="F23:I23" si="3">SUM(F2:F22)</f>
+        <v>149</v>
+      </c>
+      <c r="G23" s="22">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="H23" s="22">
+        <f t="shared" si="3"/>
+        <v>2036</v>
+      </c>
+      <c r="I23" s="22">
+        <f t="shared" si="3"/>
+        <v>23345</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15" customHeight="1">
+      <c r="B24" s="23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added latest update on 03 March
</commit_message>
<xml_diff>
--- a/data/covid-19_IT.xlsx
+++ b/data/covid-19_IT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlotorniai/repos/COVID-19-Italy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3CB642-7B92-FC4C-8E97-19E087881742}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C973E21-E112-AA4B-951F-36D4B88C0909}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="460" windowWidth="17740" windowHeight="16660" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="460" windowWidth="10080" windowHeight="16640" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="23.02" sheetId="2" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="29.02" sheetId="8" r:id="rId7"/>
     <sheet name="01.03" sheetId="9" r:id="rId8"/>
     <sheet name="02.03" sheetId="11" r:id="rId9"/>
+    <sheet name="03.03" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="31">
   <si>
     <t>Ricoverati con sintomi</t>
   </si>
@@ -749,6 +750,651 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{808290A6-5C5A-DE4A-BB0A-B87220BD4BDD}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16">
+      <c r="A1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1">
+      <c r="A2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="19">
+        <v>698</v>
+      </c>
+      <c r="C2" s="19">
+        <v>167</v>
+      </c>
+      <c r="D2" s="19">
+        <v>461</v>
+      </c>
+      <c r="E2" s="16">
+        <f t="shared" ref="E2:E23" si="0">SUM(B2:D2)</f>
+        <v>1326</v>
+      </c>
+      <c r="F2" s="19">
+        <v>139</v>
+      </c>
+      <c r="G2" s="19">
+        <v>55</v>
+      </c>
+      <c r="H2" s="16">
+        <f t="shared" ref="H2:H22" si="1">SUM(E2:G2)</f>
+        <v>1520</v>
+      </c>
+      <c r="I2" s="19">
+        <v>9577</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1">
+      <c r="A3" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="19">
+        <v>49</v>
+      </c>
+      <c r="C3" s="19">
+        <v>19</v>
+      </c>
+      <c r="D3" s="19">
+        <v>229</v>
+      </c>
+      <c r="E3" s="16">
+        <f t="shared" si="0"/>
+        <v>297</v>
+      </c>
+      <c r="F3" s="16">
+        <v>7</v>
+      </c>
+      <c r="G3" s="16">
+        <v>3</v>
+      </c>
+      <c r="H3" s="16">
+        <f t="shared" si="1"/>
+        <v>307</v>
+      </c>
+      <c r="I3" s="19">
+        <v>10176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1">
+      <c r="A4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="19">
+        <v>187</v>
+      </c>
+      <c r="C4" s="19">
+        <v>24</v>
+      </c>
+      <c r="D4" s="19">
+        <v>187</v>
+      </c>
+      <c r="E4" s="16">
+        <f t="shared" si="0"/>
+        <v>398</v>
+      </c>
+      <c r="F4" s="16">
+        <v>4</v>
+      </c>
+      <c r="G4" s="19">
+        <v>18</v>
+      </c>
+      <c r="H4" s="16">
+        <f t="shared" si="1"/>
+        <v>420</v>
+      </c>
+      <c r="I4" s="19">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1">
+      <c r="A5" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="19">
+        <v>13</v>
+      </c>
+      <c r="C5" s="19">
+        <v>3</v>
+      </c>
+      <c r="D5" s="19">
+        <v>40</v>
+      </c>
+      <c r="E5" s="16">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="I5" s="19">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1">
+      <c r="A6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="19">
+        <v>12</v>
+      </c>
+      <c r="C6" s="16">
+        <v>2</v>
+      </c>
+      <c r="D6" s="19">
+        <v>5</v>
+      </c>
+      <c r="E6" s="16">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F6" s="16">
+        <v>4</v>
+      </c>
+      <c r="G6" s="16">
+        <v>1</v>
+      </c>
+      <c r="H6" s="16">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="I6" s="16">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1">
+      <c r="A7" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="19">
+        <v>27</v>
+      </c>
+      <c r="C7" s="19">
+        <v>13</v>
+      </c>
+      <c r="D7" s="19">
+        <v>19</v>
+      </c>
+      <c r="E7" s="16">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16">
+        <v>2</v>
+      </c>
+      <c r="H7" s="16">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="I7" s="19">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1">
+      <c r="A8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="16">
+        <v>10</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="19">
+        <v>8</v>
+      </c>
+      <c r="E8" s="16">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F8" s="16">
+        <v>1</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="I8" s="19">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18">
+      <c r="A9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="16">
+        <v>2</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="19">
+        <v>3</v>
+      </c>
+      <c r="E9" s="16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F9" s="16">
+        <v>2</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I9" s="19">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1">
+      <c r="A10" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="16">
+        <v>10</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16">
+        <v>1</v>
+      </c>
+      <c r="E10" s="16">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F10" s="16">
+        <v>3</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="I10" s="19">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1">
+      <c r="A11" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="19">
+        <v>11</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="19">
+        <v>19</v>
+      </c>
+      <c r="E11" s="16">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="I11" s="16">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1">
+      <c r="A12" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="16">
+        <v>2</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16">
+        <v>4</v>
+      </c>
+      <c r="E12" s="16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I12" s="19">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1">
+      <c r="A13" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="16">
+        <v>1</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I13" s="19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1">
+      <c r="A14" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="19">
+        <v>5</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="19">
+        <v>1</v>
+      </c>
+      <c r="E14" s="16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I14" s="19">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1">
+      <c r="A15" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16">
+        <v>1</v>
+      </c>
+      <c r="E15" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I15" s="19">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15" customHeight="1">
+      <c r="A16" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I16" s="19">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15" customHeight="1">
+      <c r="A17" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="16">
+        <v>1</v>
+      </c>
+      <c r="C17" s="16">
+        <v>1</v>
+      </c>
+      <c r="D17" s="19">
+        <v>6</v>
+      </c>
+      <c r="E17" s="16">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I17" s="19">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" customHeight="1">
+      <c r="A18" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" customHeight="1">
+      <c r="A19" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="16">
+        <v>1</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="19">
+        <v>12</v>
+      </c>
+      <c r="E19" s="16">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="I19" s="19">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" customHeight="1">
+      <c r="A20" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="16">
+        <v>1</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16">
+        <v>3</v>
+      </c>
+      <c r="E20" s="16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I20" s="19">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15" customHeight="1">
+      <c r="A21" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="16">
+        <v>3</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I21" s="19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" customHeight="1" thickBot="1">
+      <c r="A22" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16">
+        <v>1</v>
+      </c>
+      <c r="E22" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I22" s="19">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15" customHeight="1" thickBot="1">
+      <c r="A23" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="21">
+        <f t="shared" ref="B23:D23" si="2">SUM(B2:B22)</f>
+        <v>1034</v>
+      </c>
+      <c r="C23" s="21">
+        <f t="shared" si="2"/>
+        <v>229</v>
+      </c>
+      <c r="D23" s="21">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+      <c r="E23" s="22">
+        <f t="shared" si="0"/>
+        <v>2263</v>
+      </c>
+      <c r="F23" s="22">
+        <f t="shared" ref="F23:I23" si="3">SUM(F2:F22)</f>
+        <v>160</v>
+      </c>
+      <c r="G23" s="22">
+        <f t="shared" si="3"/>
+        <v>79</v>
+      </c>
+      <c r="H23" s="22">
+        <f t="shared" si="3"/>
+        <v>2502</v>
+      </c>
+      <c r="I23" s="22">
+        <f t="shared" si="3"/>
+        <v>25856</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15" customHeight="1">
+      <c r="B24" s="23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5614,7 +6260,7 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Updated with 04.03 data
</commit_message>
<xml_diff>
--- a/data/covid-19_IT.xlsx
+++ b/data/covid-19_IT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlotorniai/repos/COVID-19-Italy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C973E21-E112-AA4B-951F-36D4B88C0909}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49C5F05-B608-F34F-9887-2680F772156C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="460" windowWidth="10080" windowHeight="16640" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="460" windowWidth="10000" windowHeight="16640" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="23.02" sheetId="2" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="01.03" sheetId="9" r:id="rId8"/>
     <sheet name="02.03" sheetId="11" r:id="rId9"/>
     <sheet name="03.03" sheetId="12" r:id="rId10"/>
+    <sheet name="04.03" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="31">
   <si>
     <t>Ricoverati con sintomi</t>
   </si>
@@ -760,7 +761,7 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1388,6 +1389,659 @@
       <c r="I23" s="22">
         <f t="shared" si="3"/>
         <v>25856</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15" customHeight="1">
+      <c r="B24" s="23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645F012A-EC83-254D-8E34-B9B3CD4A3D33}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16">
+      <c r="A1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1">
+      <c r="A2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="19">
+        <v>877</v>
+      </c>
+      <c r="C2" s="19">
+        <v>209</v>
+      </c>
+      <c r="D2" s="19">
+        <v>411</v>
+      </c>
+      <c r="E2" s="16">
+        <f t="shared" ref="E2:E23" si="0">SUM(B2:D2)</f>
+        <v>1497</v>
+      </c>
+      <c r="F2" s="19">
+        <v>250</v>
+      </c>
+      <c r="G2" s="19">
+        <v>73</v>
+      </c>
+      <c r="H2" s="16">
+        <f t="shared" ref="H2:H22" si="1">SUM(E2:G2)</f>
+        <v>1820</v>
+      </c>
+      <c r="I2" s="19">
+        <v>12138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1">
+      <c r="A3" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="19">
+        <v>76</v>
+      </c>
+      <c r="C3" s="19">
+        <v>23</v>
+      </c>
+      <c r="D3" s="19">
+        <v>246</v>
+      </c>
+      <c r="E3" s="16">
+        <f t="shared" si="0"/>
+        <v>345</v>
+      </c>
+      <c r="F3" s="16">
+        <v>9</v>
+      </c>
+      <c r="G3" s="16">
+        <v>6</v>
+      </c>
+      <c r="H3" s="16">
+        <f t="shared" si="1"/>
+        <v>360</v>
+      </c>
+      <c r="I3" s="19">
+        <v>10515</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1">
+      <c r="A4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="19">
+        <v>256</v>
+      </c>
+      <c r="C4" s="19">
+        <v>26</v>
+      </c>
+      <c r="D4" s="19">
+        <v>234</v>
+      </c>
+      <c r="E4" s="16">
+        <f t="shared" si="0"/>
+        <v>516</v>
+      </c>
+      <c r="F4" s="16">
+        <v>6</v>
+      </c>
+      <c r="G4" s="19">
+        <v>22</v>
+      </c>
+      <c r="H4" s="16">
+        <f t="shared" si="1"/>
+        <v>544</v>
+      </c>
+      <c r="I4" s="19">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1">
+      <c r="A5" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="19">
+        <v>26</v>
+      </c>
+      <c r="C5" s="19">
+        <v>13</v>
+      </c>
+      <c r="D5" s="19">
+        <v>43</v>
+      </c>
+      <c r="E5" s="16">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="I5" s="19">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1">
+      <c r="A6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="19">
+        <v>10</v>
+      </c>
+      <c r="C6" s="16">
+        <v>3</v>
+      </c>
+      <c r="D6" s="19">
+        <v>8</v>
+      </c>
+      <c r="E6" s="16">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="F6" s="16">
+        <v>4</v>
+      </c>
+      <c r="G6" s="16">
+        <v>1</v>
+      </c>
+      <c r="H6" s="16">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="I6" s="16">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1">
+      <c r="A7" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="19">
+        <v>34</v>
+      </c>
+      <c r="C7" s="19">
+        <v>15</v>
+      </c>
+      <c r="D7" s="19">
+        <v>31</v>
+      </c>
+      <c r="E7" s="16">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16">
+        <v>4</v>
+      </c>
+      <c r="H7" s="16">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="I7" s="19">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1">
+      <c r="A8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="16">
+        <v>15</v>
+      </c>
+      <c r="C8" s="16">
+        <v>2</v>
+      </c>
+      <c r="D8" s="19">
+        <v>20</v>
+      </c>
+      <c r="E8" s="16">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="F8" s="16">
+        <v>1</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="I8" s="19">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18">
+      <c r="A9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="16">
+        <v>5</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="19">
+        <v>11</v>
+      </c>
+      <c r="E9" s="16">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F9" s="16">
+        <v>2</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="I9" s="19">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1">
+      <c r="A10" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="16">
+        <v>15</v>
+      </c>
+      <c r="C10" s="16">
+        <v>3</v>
+      </c>
+      <c r="D10" s="16">
+        <v>9</v>
+      </c>
+      <c r="E10" s="16">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="F10" s="16">
+        <v>3</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="I10" s="19">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1">
+      <c r="A11" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="19">
+        <v>11</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="19">
+        <v>20</v>
+      </c>
+      <c r="E11" s="16">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="I11" s="16">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1">
+      <c r="A12" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="16">
+        <v>4</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16">
+        <v>3</v>
+      </c>
+      <c r="E12" s="16">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F12" s="16">
+        <v>1</v>
+      </c>
+      <c r="G12" s="16">
+        <v>1</v>
+      </c>
+      <c r="H12" s="16">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I12" s="19">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1">
+      <c r="A13" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="16">
+        <v>1</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I13" s="19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1">
+      <c r="A14" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="19">
+        <v>7</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="16">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I14" s="19">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1">
+      <c r="A15" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16">
+        <v>1</v>
+      </c>
+      <c r="E15" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I15" s="19">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15" customHeight="1">
+      <c r="A16" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I16" s="19">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15" customHeight="1">
+      <c r="A17" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="16">
+        <v>1</v>
+      </c>
+      <c r="C17" s="16">
+        <v>1</v>
+      </c>
+      <c r="D17" s="19">
+        <v>7</v>
+      </c>
+      <c r="E17" s="16">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I17" s="19">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" customHeight="1">
+      <c r="A18" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" customHeight="1">
+      <c r="A19" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="16">
+        <v>3</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="19">
+        <v>15</v>
+      </c>
+      <c r="E19" s="16">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="I19" s="19">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" customHeight="1">
+      <c r="A20" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="16">
+        <v>1</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16">
+        <v>4</v>
+      </c>
+      <c r="E20" s="16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I20" s="19">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15" customHeight="1">
+      <c r="A21" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="16">
+        <v>3</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I21" s="19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" customHeight="1" thickBot="1">
+      <c r="A22" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16">
+        <v>1</v>
+      </c>
+      <c r="E22" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I22" s="19">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15" customHeight="1" thickBot="1">
+      <c r="A23" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="21">
+        <f t="shared" ref="B23:D23" si="2">SUM(B2:B22)</f>
+        <v>1346</v>
+      </c>
+      <c r="C23" s="21">
+        <f t="shared" si="2"/>
+        <v>295</v>
+      </c>
+      <c r="D23" s="21">
+        <f t="shared" si="2"/>
+        <v>1065</v>
+      </c>
+      <c r="E23" s="22">
+        <f t="shared" si="0"/>
+        <v>2706</v>
+      </c>
+      <c r="F23" s="22">
+        <f t="shared" ref="F23:I23" si="3">SUM(F2:F22)</f>
+        <v>276</v>
+      </c>
+      <c r="G23" s="22">
+        <f t="shared" si="3"/>
+        <v>107</v>
+      </c>
+      <c r="H23" s="22">
+        <f t="shared" si="3"/>
+        <v>3089</v>
+      </c>
+      <c r="I23" s="22">
+        <f t="shared" si="3"/>
+        <v>29837</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1">

</xml_diff>

<commit_message>
Updarted todays' data extended summary wih tpercentage and percentage graph, added write of the summary on Gdrive
</commit_message>
<xml_diff>
--- a/data/covid-19_IT.xlsx
+++ b/data/covid-19_IT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlotorniai/repos/COVID-19-Italy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49C5F05-B608-F34F-9887-2680F772156C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11695C02-7BF8-394A-B896-1D528DDFB3D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="460" windowWidth="10000" windowHeight="16640" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="460" windowWidth="10000" windowHeight="16340" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="23.02" sheetId="2" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="02.03" sheetId="11" r:id="rId9"/>
     <sheet name="03.03" sheetId="12" r:id="rId10"/>
     <sheet name="04.03" sheetId="13" r:id="rId11"/>
+    <sheet name="05.03" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="31">
   <si>
     <t>Ricoverati con sintomi</t>
   </si>
@@ -297,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -331,6 +332,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1406,8 +1408,8 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="I23" sqref="I23"/>
@@ -2042,6 +2044,669 @@
       <c r="I23" s="22">
         <f t="shared" si="3"/>
         <v>29837</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15" customHeight="1">
+      <c r="B24" s="23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C173B073-9654-A54F-9394-399D4D4F8F9E}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H28" sqref="H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16">
+      <c r="A1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1">
+      <c r="A2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="19">
+        <v>1169</v>
+      </c>
+      <c r="C2" s="19">
+        <v>244</v>
+      </c>
+      <c r="D2" s="19">
+        <v>364</v>
+      </c>
+      <c r="E2" s="16">
+        <f t="shared" ref="E2:E23" si="0">SUM(B2:D2)</f>
+        <v>1777</v>
+      </c>
+      <c r="F2" s="27">
+        <v>376</v>
+      </c>
+      <c r="G2" s="19">
+        <v>98</v>
+      </c>
+      <c r="H2" s="16">
+        <f t="shared" ref="H2:H22" si="1">SUM(E2:G2)</f>
+        <v>2251</v>
+      </c>
+      <c r="I2" s="19">
+        <v>12354</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1">
+      <c r="A3" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="19">
+        <v>92</v>
+      </c>
+      <c r="C3" s="19">
+        <v>24</v>
+      </c>
+      <c r="D3" s="19">
+        <v>264</v>
+      </c>
+      <c r="E3" s="16">
+        <f t="shared" si="0"/>
+        <v>380</v>
+      </c>
+      <c r="F3" s="16">
+        <v>17</v>
+      </c>
+      <c r="G3" s="16">
+        <v>10</v>
+      </c>
+      <c r="H3" s="16">
+        <f t="shared" si="1"/>
+        <v>407</v>
+      </c>
+      <c r="I3" s="19">
+        <v>11949</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1">
+      <c r="A4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="19">
+        <v>327</v>
+      </c>
+      <c r="C4" s="19">
+        <v>32</v>
+      </c>
+      <c r="D4" s="19">
+        <v>299</v>
+      </c>
+      <c r="E4" s="16">
+        <f t="shared" si="0"/>
+        <v>658</v>
+      </c>
+      <c r="F4" s="16">
+        <v>10</v>
+      </c>
+      <c r="G4" s="19">
+        <v>30</v>
+      </c>
+      <c r="H4" s="16">
+        <f t="shared" si="1"/>
+        <v>698</v>
+      </c>
+      <c r="I4" s="19">
+        <v>2884</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1">
+      <c r="A5" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="19">
+        <v>43</v>
+      </c>
+      <c r="C5" s="19">
+        <v>17</v>
+      </c>
+      <c r="D5" s="19">
+        <v>46</v>
+      </c>
+      <c r="E5" s="16">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16">
+        <v>2</v>
+      </c>
+      <c r="H5" s="16">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="I5" s="19">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1">
+      <c r="A6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="19">
+        <v>11</v>
+      </c>
+      <c r="C6" s="16">
+        <v>3</v>
+      </c>
+      <c r="D6" s="19">
+        <v>7</v>
+      </c>
+      <c r="E6" s="16">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="F6" s="16">
+        <v>4</v>
+      </c>
+      <c r="G6" s="16">
+        <v>3</v>
+      </c>
+      <c r="H6" s="16">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="I6" s="16">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1">
+      <c r="A7" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="19">
+        <v>57</v>
+      </c>
+      <c r="C7" s="19">
+        <v>19</v>
+      </c>
+      <c r="D7" s="19">
+        <v>44</v>
+      </c>
+      <c r="E7" s="16">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16">
+        <v>4</v>
+      </c>
+      <c r="H7" s="16">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="I7" s="19">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1">
+      <c r="A8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="16">
+        <v>26</v>
+      </c>
+      <c r="C8" s="16">
+        <v>3</v>
+      </c>
+      <c r="D8" s="19">
+        <v>31</v>
+      </c>
+      <c r="E8" s="16">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="F8" s="16">
+        <v>1</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="I8" s="19">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18">
+      <c r="A9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="16">
+        <v>5</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="19">
+        <v>11</v>
+      </c>
+      <c r="E9" s="16">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F9" s="16">
+        <v>2</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="I9" s="19">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1">
+      <c r="A10" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="16">
+        <v>20</v>
+      </c>
+      <c r="C10" s="16">
+        <v>7</v>
+      </c>
+      <c r="D10" s="16">
+        <v>14</v>
+      </c>
+      <c r="E10" s="16">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="F10" s="16">
+        <v>3</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="I10" s="19">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1">
+      <c r="A11" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="19">
+        <v>12</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="19">
+        <v>33</v>
+      </c>
+      <c r="E11" s="16">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="I11" s="16">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1">
+      <c r="A12" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="16">
+        <v>5</v>
+      </c>
+      <c r="C12" s="16">
+        <v>1</v>
+      </c>
+      <c r="D12" s="16">
+        <v>6</v>
+      </c>
+      <c r="E12" s="16">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F12" s="16">
+        <v>1</v>
+      </c>
+      <c r="G12" s="16">
+        <v>1</v>
+      </c>
+      <c r="H12" s="16">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="I12" s="19">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1">
+      <c r="A13" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="16">
+        <v>1</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I13" s="19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1">
+      <c r="A14" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="19">
+        <v>8</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="16">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I14" s="19">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1">
+      <c r="A15" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="16">
+        <v>1</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16">
+        <v>1</v>
+      </c>
+      <c r="E15" s="16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I15" s="19">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15" customHeight="1">
+      <c r="A16" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="16">
+        <v>2</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I16" s="19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15" customHeight="1">
+      <c r="A17" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="16">
+        <v>1</v>
+      </c>
+      <c r="C17" s="16">
+        <v>1</v>
+      </c>
+      <c r="D17" s="19">
+        <v>7</v>
+      </c>
+      <c r="E17" s="16">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I17" s="19">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" customHeight="1">
+      <c r="A18" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16">
+        <v>2</v>
+      </c>
+      <c r="E18" s="16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I18" s="19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" customHeight="1">
+      <c r="A19" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="16">
+        <v>4</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="19">
+        <v>17</v>
+      </c>
+      <c r="E19" s="16">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="I19" s="19">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" customHeight="1">
+      <c r="A20" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="16">
+        <v>2</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16">
+        <v>5</v>
+      </c>
+      <c r="E20" s="16">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I20" s="19">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15" customHeight="1">
+      <c r="A21" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="16">
+        <v>4</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16">
+        <v>3</v>
+      </c>
+      <c r="E21" s="16">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I21" s="19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" customHeight="1" thickBot="1">
+      <c r="A22" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16">
+        <v>1</v>
+      </c>
+      <c r="E22" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I22" s="19">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15" customHeight="1" thickBot="1">
+      <c r="A23" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="21">
+        <f t="shared" ref="B23:D23" si="2">SUM(B2:B22)</f>
+        <v>1790</v>
+      </c>
+      <c r="C23" s="21">
+        <f t="shared" si="2"/>
+        <v>351</v>
+      </c>
+      <c r="D23" s="21">
+        <f t="shared" si="2"/>
+        <v>1155</v>
+      </c>
+      <c r="E23" s="22">
+        <f t="shared" si="0"/>
+        <v>3296</v>
+      </c>
+      <c r="F23" s="22">
+        <f t="shared" ref="F23:I23" si="3">SUM(F2:F22)</f>
+        <v>414</v>
+      </c>
+      <c r="G23" s="22">
+        <f t="shared" si="3"/>
+        <v>148</v>
+      </c>
+      <c r="H23" s="22">
+        <f t="shared" si="3"/>
+        <v>3858</v>
+      </c>
+      <c r="I23" s="22">
+        <f t="shared" si="3"/>
+        <v>32362</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1">

</xml_diff>

<commit_message>
Updated with 06.03 Data
</commit_message>
<xml_diff>
--- a/data/covid-19_IT.xlsx
+++ b/data/covid-19_IT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlotorniai/repos/COVID-19-Italy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11695C02-7BF8-394A-B896-1D528DDFB3D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EE6D66-E817-DF49-867C-6B34A4E87545}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="460" windowWidth="10000" windowHeight="16340" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="460" windowWidth="11540" windowHeight="16340" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="23.02" sheetId="2" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="03.03" sheetId="12" r:id="rId10"/>
     <sheet name="04.03" sheetId="13" r:id="rId11"/>
     <sheet name="05.03" sheetId="14" r:id="rId12"/>
+    <sheet name="06.03" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="31">
   <si>
     <t>Ricoverati con sintomi</t>
   </si>
@@ -2061,11 +2062,11 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H28" sqref="H28"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -2707,6 +2708,676 @@
       <c r="I23" s="22">
         <f t="shared" si="3"/>
         <v>32362</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15" customHeight="1">
+      <c r="B24" s="23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92C04092-161D-0F4F-8E81-B396A8376353}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16">
+      <c r="A1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1">
+      <c r="A2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="19">
+        <v>1622</v>
+      </c>
+      <c r="C2" s="19">
+        <v>309</v>
+      </c>
+      <c r="D2" s="19">
+        <v>77</v>
+      </c>
+      <c r="E2" s="16">
+        <f t="shared" ref="E2:E23" si="0">SUM(B2:D2)</f>
+        <v>2008</v>
+      </c>
+      <c r="F2" s="27">
+        <v>469</v>
+      </c>
+      <c r="G2" s="19">
+        <v>135</v>
+      </c>
+      <c r="H2" s="16">
+        <f t="shared" ref="H2:H22" si="1">SUM(E2:G2)</f>
+        <v>2612</v>
+      </c>
+      <c r="I2" s="19">
+        <v>13556</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1">
+      <c r="A3" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="19">
+        <v>117</v>
+      </c>
+      <c r="C3" s="19">
+        <v>27</v>
+      </c>
+      <c r="D3" s="19">
+        <v>310</v>
+      </c>
+      <c r="E3" s="16">
+        <f t="shared" si="0"/>
+        <v>454</v>
+      </c>
+      <c r="F3" s="16">
+        <v>22</v>
+      </c>
+      <c r="G3" s="16">
+        <v>12</v>
+      </c>
+      <c r="H3" s="16">
+        <f t="shared" si="1"/>
+        <v>488</v>
+      </c>
+      <c r="I3" s="19">
+        <v>13023</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1">
+      <c r="A4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="19">
+        <v>397</v>
+      </c>
+      <c r="C4" s="19">
+        <v>53</v>
+      </c>
+      <c r="D4" s="19">
+        <v>366</v>
+      </c>
+      <c r="E4" s="16">
+        <f t="shared" si="0"/>
+        <v>816</v>
+      </c>
+      <c r="F4" s="16">
+        <v>17</v>
+      </c>
+      <c r="G4" s="19">
+        <v>37</v>
+      </c>
+      <c r="H4" s="16">
+        <f t="shared" si="1"/>
+        <v>870</v>
+      </c>
+      <c r="I4" s="19">
+        <v>3136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1">
+      <c r="A5" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="19">
+        <v>57</v>
+      </c>
+      <c r="C5" s="19">
+        <v>30</v>
+      </c>
+      <c r="D5" s="19">
+        <v>52</v>
+      </c>
+      <c r="E5" s="16">
+        <v>139</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16">
+        <v>4</v>
+      </c>
+      <c r="H5" s="16">
+        <f t="shared" si="1"/>
+        <v>143</v>
+      </c>
+      <c r="I5" s="19">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1">
+      <c r="A6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="19">
+        <v>12</v>
+      </c>
+      <c r="C6" s="16">
+        <v>5</v>
+      </c>
+      <c r="D6" s="19">
+        <v>7</v>
+      </c>
+      <c r="E6" s="16">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="F6" s="16">
+        <v>5</v>
+      </c>
+      <c r="G6" s="16">
+        <v>3</v>
+      </c>
+      <c r="H6" s="16">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="I6" s="16">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1">
+      <c r="A7" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="19">
+        <v>73</v>
+      </c>
+      <c r="C7" s="19">
+        <v>20</v>
+      </c>
+      <c r="D7" s="19">
+        <v>62</v>
+      </c>
+      <c r="E7" s="16">
+        <f t="shared" si="0"/>
+        <v>155</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16">
+        <v>4</v>
+      </c>
+      <c r="H7" s="16">
+        <f t="shared" si="1"/>
+        <v>159</v>
+      </c>
+      <c r="I7" s="19">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1">
+      <c r="A8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="16">
+        <v>35</v>
+      </c>
+      <c r="C8" s="16">
+        <v>5</v>
+      </c>
+      <c r="D8" s="19">
+        <v>38</v>
+      </c>
+      <c r="E8" s="16">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="F8" s="16">
+        <v>1</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="I8" s="19">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18">
+      <c r="A9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="16">
+        <v>7</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="19">
+        <v>15</v>
+      </c>
+      <c r="E9" s="16">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="F9" s="16">
+        <v>2</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="I9" s="19">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1">
+      <c r="A10" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="16">
+        <v>26</v>
+      </c>
+      <c r="C10" s="16">
+        <v>8</v>
+      </c>
+      <c r="D10" s="16">
+        <v>16</v>
+      </c>
+      <c r="E10" s="16">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="F10" s="16">
+        <v>3</v>
+      </c>
+      <c r="G10" s="16">
+        <v>1</v>
+      </c>
+      <c r="H10" s="16">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="I10" s="19">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1">
+      <c r="A11" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="19">
+        <v>12</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="19">
+        <v>45</v>
+      </c>
+      <c r="E11" s="16">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="I11" s="16">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1">
+      <c r="A12" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="16">
+        <v>5</v>
+      </c>
+      <c r="C12" s="16">
+        <v>1</v>
+      </c>
+      <c r="D12" s="16">
+        <v>9</v>
+      </c>
+      <c r="E12" s="16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F12" s="16">
+        <v>1</v>
+      </c>
+      <c r="G12" s="16">
+        <v>1</v>
+      </c>
+      <c r="H12" s="16">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="I12" s="19">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1">
+      <c r="A13" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="16">
+        <v>4</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I13" s="19">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1">
+      <c r="A14" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="19">
+        <v>9</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="16">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I14" s="19">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1">
+      <c r="A15" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="16">
+        <v>2</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16">
+        <v>2</v>
+      </c>
+      <c r="E15" s="16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I15" s="19">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15" customHeight="1">
+      <c r="A16" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="16">
+        <v>2</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16">
+        <v>3</v>
+      </c>
+      <c r="E16" s="16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I16" s="19">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15" customHeight="1">
+      <c r="A17" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="16">
+        <v>2</v>
+      </c>
+      <c r="C17" s="16">
+        <v>2</v>
+      </c>
+      <c r="D17" s="19">
+        <v>12</v>
+      </c>
+      <c r="E17" s="16">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="I17" s="19">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" customHeight="1">
+      <c r="A18" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16">
+        <v>7</v>
+      </c>
+      <c r="E18" s="16">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I18" s="19">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" customHeight="1">
+      <c r="A19" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="16">
+        <v>4</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="19">
+        <v>24</v>
+      </c>
+      <c r="E19" s="16">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="F19" s="16">
+        <v>3</v>
+      </c>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="I19" s="19">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" customHeight="1">
+      <c r="A20" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="16">
+        <v>4</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16">
+        <v>6</v>
+      </c>
+      <c r="E20" s="16">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I20" s="19">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15" customHeight="1">
+      <c r="A21" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="16">
+        <v>3</v>
+      </c>
+      <c r="C21" s="16">
+        <v>2</v>
+      </c>
+      <c r="D21" s="16">
+        <v>7</v>
+      </c>
+      <c r="E21" s="16">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="I21" s="19">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" customHeight="1" thickBot="1">
+      <c r="A22" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="16">
+        <v>1</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16">
+        <v>2</v>
+      </c>
+      <c r="E22" s="16">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I22" s="19">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15" customHeight="1" thickBot="1">
+      <c r="A23" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="21">
+        <f t="shared" ref="B23:D23" si="2">SUM(B2:B22)</f>
+        <v>2394</v>
+      </c>
+      <c r="C23" s="21">
+        <f t="shared" si="2"/>
+        <v>462</v>
+      </c>
+      <c r="D23" s="21">
+        <f t="shared" si="2"/>
+        <v>1060</v>
+      </c>
+      <c r="E23" s="22">
+        <f t="shared" si="0"/>
+        <v>3916</v>
+      </c>
+      <c r="F23" s="22">
+        <f t="shared" ref="F23:I23" si="3">SUM(F2:F22)</f>
+        <v>523</v>
+      </c>
+      <c r="G23" s="22">
+        <f t="shared" si="3"/>
+        <v>197</v>
+      </c>
+      <c r="H23" s="22">
+        <f t="shared" si="3"/>
+        <v>4636</v>
+      </c>
+      <c r="I23" s="22">
+        <f t="shared" si="3"/>
+        <v>36359</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1">

</xml_diff>